<commit_message>
Apache POI dependency has been added to the pom.xml file in order to manipulate excel Microsoft Office files.
First study: ExcelRead.java
</commit_message>
<xml_diff>
--- a/Sample_excel.xlsx
+++ b/Sample_excel.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/burakarikboga/Desktop/SDET_EU8/4. Test Automation/Projects/cucumber-junit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FBE221-1E71-7047-8D9A-6BE919C30264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C966D786-0EF6-A34E-9BCE-840B090C3C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{A46882D5-2A86-C74C-9341-0F14D0803863}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Employees" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,9 +32,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>value</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>Vinod</t>
+  </si>
+  <si>
+    <t>Mansoor</t>
+  </si>
+  <si>
+    <t>Linda</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Kumar</t>
+  </si>
+  <si>
+    <t>Khan</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>Job_Title</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>PO</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>Developer</t>
   </si>
 </sst>
 </file>
@@ -386,17 +431,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D92FE74-F71F-5F40-B8DA-560B345ECF69}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
VyTrackLoginPage has been tested by using DDT. Credentials are read from an .xlxs file and used in tests and finally the test result have been written in same .xlxs file.
Last practice: VyTrackLoginDDTTest.java
</commit_message>
<xml_diff>
--- a/Sample_excel.xlsx
+++ b/Sample_excel.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/burakarikboga/Desktop/SDET_EU8/4. Test Automation/Projects/cucumber-junit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78EF7D2-F9B2-F146-ADBC-9069BAA27610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94C3BD4-E77C-F44C-B482-1030D53B8E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{A46882D5-2A86-C74C-9341-0F14D0803863}"/>
+    <workbookView xWindow="18620" yWindow="2200" windowWidth="16340" windowHeight="17440" activeTab="1" xr2:uid="{A46882D5-2A86-C74C-9341-0F14D0803863}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
+    <sheet name="VyTrackQA2User" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>FirstName</t>
   </si>
@@ -83,6 +84,69 @@
   </si>
   <si>
     <t>Salary</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>UserUser123</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>user2</t>
+  </si>
+  <si>
+    <t>Bella</t>
+  </si>
+  <si>
+    <t>Stamm</t>
+  </si>
+  <si>
+    <t>storemanager51</t>
+  </si>
+  <si>
+    <t>Edd</t>
+  </si>
+  <si>
+    <t>Turner</t>
+  </si>
+  <si>
+    <t>Roma</t>
+  </si>
+  <si>
+    <t>Medhurst</t>
+  </si>
+  <si>
+    <t>storemanager52</t>
+  </si>
+  <si>
+    <t>storemanager101</t>
+  </si>
+  <si>
+    <t>storemanager102</t>
   </si>
 </sst>
 </file>
@@ -437,13 +501,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D92FE74-F71F-5F40-B8DA-560B345ECF69}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,7 +524,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -473,11 +537,11 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" t="n">
-        <v>200000.0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -490,11 +554,11 @@
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="E3" t="n">
-        <v>190000.0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>190000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -507,11 +571,11 @@
       <c r="D4">
         <v>3</v>
       </c>
-      <c r="E4" t="n">
-        <v>175000.0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>175000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -524,8 +588,146 @@
       <c r="D5">
         <v>4</v>
       </c>
-      <c r="E5" t="n">
-        <v>210000.0</v>
+      <c r="E5">
+        <v>210000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B01C488-DF6E-4C4A-856D-B449497D4E35}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="218" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.6640625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.83203125"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
VyTrackLoginPage has been tested by using DDT. Credentials are read from an .xlsx file and used in tests and finally the test result have been written in same .xlsx file.
Last practice: VyTrackLoginDDTTest.java
</commit_message>
<xml_diff>
--- a/Sample_excel.xlsx
+++ b/Sample_excel.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/burakarikboga/Desktop/SDET_EU8/4. Test Automation/Projects/cucumber-junit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E78EF7D2-F9B2-F146-ADBC-9069BAA27610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94C3BD4-E77C-F44C-B482-1030D53B8E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{A46882D5-2A86-C74C-9341-0F14D0803863}"/>
+    <workbookView xWindow="18620" yWindow="2200" windowWidth="16340" windowHeight="17440" activeTab="1" xr2:uid="{A46882D5-2A86-C74C-9341-0F14D0803863}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
+    <sheet name="VyTrackQA2User" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>FirstName</t>
   </si>
@@ -83,6 +84,69 @@
   </si>
   <si>
     <t>Salary</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>UserUser123</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>user2</t>
+  </si>
+  <si>
+    <t>Bella</t>
+  </si>
+  <si>
+    <t>Stamm</t>
+  </si>
+  <si>
+    <t>storemanager51</t>
+  </si>
+  <si>
+    <t>Edd</t>
+  </si>
+  <si>
+    <t>Turner</t>
+  </si>
+  <si>
+    <t>Roma</t>
+  </si>
+  <si>
+    <t>Medhurst</t>
+  </si>
+  <si>
+    <t>storemanager52</t>
+  </si>
+  <si>
+    <t>storemanager101</t>
+  </si>
+  <si>
+    <t>storemanager102</t>
   </si>
 </sst>
 </file>
@@ -437,13 +501,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D92FE74-F71F-5F40-B8DA-560B345ECF69}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,7 +524,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -473,11 +537,11 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" t="n">
-        <v>200000.0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -490,11 +554,11 @@
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="E3" t="n">
-        <v>190000.0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>190000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -507,11 +571,11 @@
       <c r="D4">
         <v>3</v>
       </c>
-      <c r="E4" t="n">
-        <v>175000.0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>175000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -524,8 +588,146 @@
       <c r="D5">
         <v>4</v>
       </c>
-      <c r="E5" t="n">
-        <v>210000.0</v>
+      <c r="E5">
+        <v>210000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B01C488-DF6E-4C4A-856D-B449497D4E35}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="218" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.6640625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.83203125"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>